<commit_message>
Update return period with 50 years data
</commit_message>
<xml_diff>
--- a/oddrin/raster.xlsx
+++ b/oddrin/raster.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="358" uniqueCount="241">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="239">
   <si>
     <t xml:space="preserve">Country name</t>
   </si>
@@ -34,6 +34,9 @@
     <t xml:space="preserve">Return_Period_25_Years</t>
   </si>
   <si>
+    <t xml:space="preserve">Return_Period_50_Years</t>
+  </si>
+  <si>
     <t xml:space="preserve">China</t>
   </si>
   <si>
@@ -55,12 +58,6 @@
     <t xml:space="preserve">IDN</t>
   </si>
   <si>
-    <t xml:space="preserve">Russia</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RUS</t>
-  </si>
-  <si>
     <t xml:space="preserve">Dem. Rep. Congo</t>
   </si>
   <si>
@@ -397,12 +394,6 @@
     <t xml:space="preserve">LAO</t>
   </si>
   <si>
-    <t xml:space="preserve">Dem. People's Rep. Korea</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PRK</t>
-  </si>
-  <si>
     <t xml:space="preserve">Serbia</t>
   </si>
   <si>
@@ -517,6 +508,9 @@
     <t xml:space="preserve">MRT</t>
   </si>
   <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
     <t xml:space="preserve">Senegal</t>
   </si>
   <si>
@@ -547,12 +541,6 @@
     <t xml:space="preserve">PRT</t>
   </si>
   <si>
-    <t xml:space="preserve">Taiwan, China</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TWN</t>
-  </si>
-  <si>
     <t xml:space="preserve">Guyana</t>
   </si>
   <si>
@@ -743,6 +731,12 @@
   </si>
   <si>
     <t xml:space="preserve">QAT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ireland</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IRL</t>
   </si>
 </sst>
 </file>
@@ -752,7 +746,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="8">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -789,8 +783,19 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -807,6 +812,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FF3465A4"/>
         <bgColor rgb="FF3366FF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF168253"/>
+        <bgColor rgb="FF008080"/>
       </patternFill>
     </fill>
     <fill>
@@ -850,7 +861,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -867,15 +878,23 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -903,7 +922,7 @@
       <rgbColor rgb="FF000080"/>
       <rgbColor rgb="FF808000"/>
       <rgbColor rgb="FF800080"/>
-      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FF168253"/>
       <rgbColor rgb="FFC0C0C0"/>
       <rgbColor rgb="FF808080"/>
       <rgbColor rgb="FF5B9BD5"/>
@@ -956,10 +975,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D119"/>
+  <dimension ref="A1:F117"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A25" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B49" activeCellId="0" sqref="B49"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A85" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E107" activeCellId="0" sqref="E107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -968,6 +987,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="45.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="40.69"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="26.81"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="31.4"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -983,1654 +1003,1983 @@
       <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
+      <c r="E1" s="4" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="4" t="s">
+      <c r="A2" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="B2" s="5" t="s">
         <v>6</v>
       </c>
+      <c r="C2" s="5" t="s">
+        <v>7</v>
+      </c>
       <c r="D2" s="0" t="n">
-        <v>3967718</v>
+        <v>973310</v>
+      </c>
+      <c r="E2" s="0" t="n">
+        <v>1804655</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" s="6" t="s">
+      <c r="A3" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="4" t="s">
-        <v>6</v>
+      <c r="B3" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>7</v>
       </c>
       <c r="D3" s="0" t="n">
-        <v>5204462</v>
+        <v>1361165</v>
+      </c>
+      <c r="E3" s="0" t="n">
+        <v>1594930</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" s="6" t="s">
+      <c r="A4" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="4" t="s">
-        <v>6</v>
+      <c r="B4" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>7</v>
       </c>
       <c r="D4" s="0" t="n">
-        <v>2022163</v>
+        <v>321919</v>
+      </c>
+      <c r="E4" s="0" t="n">
+        <v>429722</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="B5" s="6" t="s">
+      <c r="A5" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="4" t="s">
-        <v>6</v>
+      <c r="B5" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" s="0" t="n">
+        <v>407575</v>
+      </c>
+      <c r="E5" s="0" t="n">
+        <v>441053</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B6" s="6" t="s">
+      <c r="A6" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="4" t="s">
-        <v>6</v>
+      <c r="B6" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>7</v>
       </c>
       <c r="D6" s="0" t="n">
-        <v>1342248</v>
+        <v>1734354</v>
+      </c>
+      <c r="E6" s="0" t="n">
+        <v>2017090</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="B7" s="6" t="s">
+      <c r="A7" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="C7" s="4" t="s">
-        <v>6</v>
+      <c r="B7" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>7</v>
       </c>
       <c r="D7" s="0" t="n">
-        <v>3836094</v>
+        <v>312885</v>
+      </c>
+      <c r="E7" s="0" t="n">
+        <v>333364</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="B8" s="6" t="s">
+      <c r="A8" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="C8" s="4" t="s">
-        <v>6</v>
+      <c r="B8" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>7</v>
       </c>
       <c r="D8" s="0" t="n">
-        <v>3581593</v>
+        <v>177572</v>
+      </c>
+      <c r="E8" s="0" t="n">
+        <v>191977</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="B9" s="6" t="s">
+      <c r="A9" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="C9" s="4" t="s">
-        <v>6</v>
+      <c r="B9" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>7</v>
       </c>
       <c r="D9" s="0" t="n">
-        <v>1021619</v>
+        <v>167246</v>
+      </c>
+      <c r="E9" s="0" t="n">
+        <v>332493</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="B10" s="6" t="s">
+      <c r="A10" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="C10" s="4" t="s">
-        <v>6</v>
+      <c r="B10" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>7</v>
       </c>
       <c r="D10" s="0" t="n">
-        <v>1376429</v>
+        <v>339560</v>
+      </c>
+      <c r="E10" s="0" t="n">
+        <v>422674</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="B11" s="6" t="s">
+      <c r="A11" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="C11" s="4" t="s">
-        <v>6</v>
+      <c r="B11" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>7</v>
       </c>
       <c r="D11" s="0" t="n">
-        <v>3853963</v>
+        <v>226540</v>
+      </c>
+      <c r="E11" s="0" t="n">
+        <v>236633</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="B12" s="6" t="s">
+      <c r="A12" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="C12" s="4" t="s">
-        <v>6</v>
+      <c r="B12" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>7</v>
       </c>
       <c r="D12" s="0" t="n">
-        <v>1000413</v>
+        <v>17686</v>
+      </c>
+      <c r="E12" s="0" t="n">
+        <v>18943</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="B13" s="6" t="s">
+      <c r="A13" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="C13" s="4" t="s">
-        <v>6</v>
+      <c r="B13" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>7</v>
       </c>
       <c r="D13" s="0" t="n">
-        <v>103873</v>
+        <v>137832</v>
+      </c>
+      <c r="E13" s="0" t="n">
+        <v>192849</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="B14" s="6" t="s">
+      <c r="A14" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="C14" s="4" t="s">
-        <v>6</v>
+      <c r="B14" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>7</v>
       </c>
       <c r="D14" s="0" t="n">
-        <v>1629708</v>
+        <v>510557</v>
+      </c>
+      <c r="E14" s="0" t="n">
+        <v>784211</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="B15" s="6" t="s">
+      <c r="A15" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="C15" s="4" t="s">
-        <v>6</v>
+      <c r="B15" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>7</v>
       </c>
       <c r="D15" s="0" t="n">
-        <v>2778557</v>
+        <v>553011</v>
+      </c>
+      <c r="E15" s="0" t="n">
+        <v>592652</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="B16" s="6" t="s">
+      <c r="A16" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="C16" s="4" t="s">
-        <v>6</v>
+      <c r="B16" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>7</v>
       </c>
       <c r="D16" s="0" t="n">
-        <v>4266242</v>
+        <v>84146</v>
+      </c>
+      <c r="E16" s="0" t="n">
+        <v>285001</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="B17" s="6" t="s">
+      <c r="A17" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="C17" s="4" t="s">
-        <v>6</v>
+      <c r="B17" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>7</v>
       </c>
       <c r="D17" s="0" t="n">
-        <v>2803628</v>
+        <v>778765</v>
+      </c>
+      <c r="E17" s="0" t="n">
+        <v>886569</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="B18" s="6" t="s">
+      <c r="A18" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="C18" s="4" t="s">
-        <v>6</v>
+      <c r="B18" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>7</v>
       </c>
       <c r="D18" s="0" t="n">
-        <v>7886488</v>
+        <v>31732</v>
+      </c>
+      <c r="E18" s="0" t="n">
+        <v>41596</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="B19" s="6" t="s">
+      <c r="A19" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="C19" s="4" t="s">
-        <v>6</v>
+      <c r="B19" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>7</v>
       </c>
       <c r="D19" s="0" t="n">
-        <v>261012</v>
+        <v>69266</v>
+      </c>
+      <c r="E19" s="0" t="n">
+        <v>101142</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="B20" s="6" t="s">
+      <c r="A20" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="C20" s="4" t="s">
-        <v>6</v>
+      <c r="B20" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>7</v>
       </c>
       <c r="D20" s="0" t="n">
-        <v>417595</v>
+        <v>310097</v>
+      </c>
+      <c r="E20" s="0" t="n">
+        <v>361680</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="B21" s="6" t="s">
+      <c r="A21" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="C21" s="4" t="s">
-        <v>6</v>
+      <c r="B21" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>7</v>
       </c>
       <c r="D21" s="0" t="n">
-        <v>1566781</v>
+        <v>158097</v>
+      </c>
+      <c r="E21" s="0" t="n">
+        <v>208883</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="B22" s="6" t="s">
+      <c r="A22" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="C22" s="4" t="s">
-        <v>6</v>
+      <c r="B22" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>7</v>
       </c>
       <c r="D22" s="0" t="n">
-        <v>2407051</v>
+        <v>34232</v>
+      </c>
+      <c r="E22" s="0" t="n">
+        <v>99120</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="B23" s="6" t="s">
+      <c r="A23" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="C23" s="4" t="s">
-        <v>6</v>
+      <c r="B23" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>7</v>
       </c>
       <c r="D23" s="0" t="n">
-        <v>784175</v>
+        <v>95639</v>
+      </c>
+      <c r="E23" s="0" t="n">
+        <v>103019</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="B24" s="6" t="s">
+      <c r="A24" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="C24" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D24" s="0" t="n">
-        <v>1917520</v>
+      <c r="B24" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D24" s="8" t="n">
+        <v>42208</v>
+      </c>
+      <c r="E24" s="0" t="n">
+        <v>106825</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="B25" s="6" t="s">
+      <c r="A25" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="C25" s="4" t="s">
-        <v>6</v>
+      <c r="B25" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>7</v>
       </c>
       <c r="D25" s="0" t="n">
-        <v>2245226</v>
+        <v>189939</v>
+      </c>
+      <c r="E25" s="0" t="n">
+        <v>1403555</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="B26" s="6" t="s">
+      <c r="A26" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="C26" s="4" t="s">
-        <v>6</v>
+      <c r="B26" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>7</v>
       </c>
       <c r="D26" s="0" t="n">
-        <v>7273741</v>
+        <v>382210</v>
+      </c>
+      <c r="E26" s="0" t="n">
+        <v>428405</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="B27" s="6" t="s">
+      <c r="A27" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="C27" s="4" t="s">
-        <v>6</v>
+      <c r="B27" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="C27" s="5" t="s">
+        <v>7</v>
       </c>
       <c r="D27" s="0" t="n">
-        <v>1155297</v>
+        <v>21484</v>
+      </c>
+      <c r="E27" s="0" t="n">
+        <v>30024</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="B28" s="6" t="s">
+      <c r="A28" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="C28" s="4" t="s">
-        <v>6</v>
+      <c r="B28" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="C28" s="5" t="s">
+        <v>7</v>
       </c>
       <c r="D28" s="0" t="n">
-        <v>576321</v>
+        <v>37012</v>
+      </c>
+      <c r="E28" s="0" t="n">
+        <v>53059</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="B29" s="6" t="s">
+      <c r="A29" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="C29" s="4" t="s">
-        <v>6</v>
+      <c r="B29" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="C29" s="5" t="s">
+        <v>7</v>
       </c>
       <c r="D29" s="0" t="n">
-        <v>4776829</v>
+        <v>532819</v>
+      </c>
+      <c r="E29" s="0" t="n">
+        <v>1289153</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="B30" s="6" t="s">
+      <c r="A30" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="C30" s="4" t="s">
-        <v>6</v>
+      <c r="B30" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="C30" s="5" t="s">
+        <v>7</v>
       </c>
       <c r="D30" s="0" t="n">
-        <v>3196478</v>
+        <v>295347</v>
+      </c>
+      <c r="E30" s="0" t="n">
+        <v>377502</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="B31" s="6" t="s">
+      <c r="A31" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="C31" s="4" t="s">
-        <v>6</v>
+      <c r="B31" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="C31" s="5" t="s">
+        <v>7</v>
       </c>
       <c r="D31" s="0" t="n">
-        <v>1301675</v>
+        <v>192187</v>
+      </c>
+      <c r="E31" s="0" t="n">
+        <v>473918</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="B32" s="6" t="s">
+      <c r="A32" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="C32" s="4" t="s">
-        <v>6</v>
+      <c r="B32" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="C32" s="5" t="s">
+        <v>7</v>
       </c>
       <c r="D32" s="0" t="n">
-        <v>1262100</v>
+        <v>255355</v>
+      </c>
+      <c r="E32" s="0" t="n">
+        <v>294741</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="B33" s="6" t="s">
+      <c r="A33" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="C33" s="4" t="s">
-        <v>6</v>
+      <c r="B33" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="C33" s="5" t="s">
+        <v>7</v>
       </c>
       <c r="D33" s="0" t="n">
-        <v>1933630</v>
+        <v>490800</v>
+      </c>
+      <c r="E33" s="0" t="n">
+        <v>639433</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="B34" s="6" t="s">
+      <c r="A34" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="C34" s="4" t="s">
-        <v>6</v>
+      <c r="B34" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="C34" s="5" t="s">
+        <v>7</v>
       </c>
       <c r="D34" s="0" t="n">
-        <v>2381657</v>
+        <v>206914</v>
+      </c>
+      <c r="E34" s="0" t="n">
+        <v>221032</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="B35" s="6" t="s">
+      <c r="A35" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="C35" s="4" t="s">
-        <v>6</v>
+      <c r="B35" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="C35" s="5" t="s">
+        <v>7</v>
       </c>
       <c r="D35" s="0" t="n">
-        <v>1604843</v>
+        <v>81286</v>
+      </c>
+      <c r="E35" s="0" t="n">
+        <v>103470</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="B36" s="6" t="s">
+      <c r="A36" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="C36" s="4" t="s">
-        <v>6</v>
+      <c r="B36" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="C36" s="5" t="s">
+        <v>7</v>
       </c>
       <c r="D36" s="0" t="n">
-        <v>308464</v>
+        <v>60463</v>
+      </c>
+      <c r="E36" s="0" t="n">
+        <v>96956</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="B37" s="6" t="s">
+      <c r="A37" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="C37" s="4" t="s">
-        <v>6</v>
+      <c r="B37" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="C37" s="5" t="s">
+        <v>7</v>
       </c>
       <c r="D37" s="0" t="n">
-        <v>442322</v>
+        <v>115274</v>
+      </c>
+      <c r="E37" s="0" t="n">
+        <v>191317</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="B38" s="6" t="s">
+      <c r="A38" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="C38" s="4" t="s">
-        <v>6</v>
+      <c r="B38" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="C38" s="5" t="s">
+        <v>7</v>
       </c>
       <c r="D38" s="0" t="n">
-        <v>834010</v>
+        <v>197225</v>
+      </c>
+      <c r="E38" s="0" t="n">
+        <v>214736</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="B39" s="6" t="s">
+      <c r="A39" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="C39" s="4" t="s">
-        <v>6</v>
+      <c r="B39" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="C39" s="5" t="s">
+        <v>7</v>
       </c>
       <c r="D39" s="0" t="n">
-        <v>2507033</v>
+        <v>269294</v>
+      </c>
+      <c r="E39" s="0" t="n">
+        <v>378269</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="B40" s="6" t="s">
+      <c r="A40" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="C40" s="4" t="s">
-        <v>6</v>
+      <c r="B40" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="C40" s="5" t="s">
+        <v>7</v>
       </c>
       <c r="D40" s="0" t="n">
-        <v>3467059</v>
+        <v>162247</v>
+      </c>
+      <c r="E40" s="0" t="n">
+        <v>242280</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="B41" s="6" t="s">
+      <c r="A41" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="C41" s="4" t="s">
-        <v>6</v>
+      <c r="B41" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="C41" s="5" t="s">
+        <v>7</v>
       </c>
       <c r="D41" s="0" t="n">
-        <v>2387476</v>
+        <v>432675</v>
+      </c>
+      <c r="E41" s="0" t="n">
+        <v>571061</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="B42" s="6" t="s">
+      <c r="A42" s="6" t="s">
         <v>86</v>
       </c>
-      <c r="C42" s="4" t="s">
-        <v>6</v>
+      <c r="B42" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="C42" s="5" t="s">
+        <v>7</v>
       </c>
       <c r="D42" s="0" t="n">
-        <v>2597166</v>
+        <v>27866</v>
+      </c>
+      <c r="E42" s="0" t="n">
+        <v>47235</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="B43" s="6" t="s">
+      <c r="A43" s="6" t="s">
         <v>88</v>
       </c>
-      <c r="C43" s="4" t="s">
-        <v>6</v>
+      <c r="B43" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="C43" s="5" t="s">
+        <v>7</v>
       </c>
       <c r="D43" s="0" t="n">
-        <v>291407</v>
+        <v>36227</v>
+      </c>
+      <c r="E43" s="0" t="n">
+        <v>36436</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="B44" s="6" t="s">
+      <c r="A44" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="C44" s="4" t="s">
-        <v>6</v>
+      <c r="B44" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="C44" s="5" t="s">
+        <v>7</v>
       </c>
       <c r="D44" s="0" t="n">
-        <v>860808</v>
+        <v>12582</v>
+      </c>
+      <c r="E44" s="0" t="n">
+        <v>379037</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="5" t="s">
-        <v>91</v>
-      </c>
-      <c r="B45" s="6" t="s">
+      <c r="A45" s="6" t="s">
         <v>92</v>
       </c>
-      <c r="C45" s="4" t="s">
-        <v>6</v>
+      <c r="B45" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="C45" s="5" t="s">
+        <v>7</v>
       </c>
       <c r="D45" s="0" t="n">
-        <v>5724828</v>
+        <v>133954</v>
+      </c>
+      <c r="E45" s="0" t="n">
+        <v>185911</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="5" t="s">
-        <v>93</v>
-      </c>
-      <c r="B46" s="6" t="s">
+      <c r="A46" s="6" t="s">
         <v>94</v>
       </c>
-      <c r="C46" s="4" t="s">
-        <v>6</v>
+      <c r="B46" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="C46" s="5" t="s">
+        <v>7</v>
       </c>
       <c r="D46" s="0" t="n">
-        <v>485860</v>
+        <v>41163</v>
+      </c>
+      <c r="E46" s="0" t="n">
+        <v>128257</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="5" t="s">
-        <v>95</v>
-      </c>
-      <c r="B47" s="6" t="s">
+      <c r="A47" s="6" t="s">
         <v>96</v>
       </c>
-      <c r="C47" s="4" t="s">
-        <v>6</v>
+      <c r="B47" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="C47" s="5" t="s">
+        <v>7</v>
       </c>
       <c r="D47" s="0" t="n">
-        <v>196221</v>
+        <v>389768</v>
+      </c>
+      <c r="E47" s="0" t="n">
+        <v>466428</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="B48" s="6" t="s">
+      <c r="A48" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="C48" s="4" t="s">
-        <v>6</v>
+      <c r="B48" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="C48" s="5" t="s">
+        <v>7</v>
       </c>
       <c r="D48" s="0" t="n">
-        <v>5410015</v>
+        <v>21090</v>
+      </c>
+      <c r="E48" s="0" t="n">
+        <v>23386</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="5" t="s">
-        <v>99</v>
-      </c>
-      <c r="B49" s="6" t="s">
+      <c r="A49" s="6" t="s">
         <v>100</v>
       </c>
-      <c r="C49" s="4" t="s">
-        <v>6</v>
+      <c r="B49" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="C49" s="5" t="s">
+        <v>7</v>
       </c>
       <c r="D49" s="0" t="n">
-        <v>178453</v>
+        <v>22811</v>
+      </c>
+      <c r="E49" s="0" t="n">
+        <v>331795</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="5" t="s">
-        <v>101</v>
-      </c>
-      <c r="B50" s="6" t="s">
+      <c r="A50" s="6" t="s">
         <v>102</v>
       </c>
-      <c r="C50" s="4" t="s">
-        <v>6</v>
+      <c r="B50" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="C50" s="5" t="s">
+        <v>7</v>
       </c>
       <c r="D50" s="0" t="n">
-        <v>2748059</v>
+        <v>269841</v>
+      </c>
+      <c r="E50" s="0" t="n">
+        <v>617916</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="5" t="s">
-        <v>103</v>
-      </c>
-      <c r="B51" s="6" t="s">
+      <c r="A51" s="6" t="s">
         <v>104</v>
       </c>
-      <c r="C51" s="4" t="s">
-        <v>6</v>
+      <c r="B51" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="C51" s="5" t="s">
+        <v>7</v>
       </c>
       <c r="D51" s="0" t="n">
-        <v>3438053</v>
+        <v>179511</v>
+      </c>
+      <c r="E51" s="0" t="n">
+        <v>197833</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="5" t="s">
-        <v>105</v>
-      </c>
-      <c r="B52" s="6" t="s">
+      <c r="A52" s="6" t="s">
         <v>106</v>
       </c>
-      <c r="C52" s="4" t="s">
-        <v>6</v>
+      <c r="B52" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="C52" s="5" t="s">
+        <v>7</v>
       </c>
       <c r="D52" s="0" t="n">
-        <v>2001489</v>
+        <v>4859</v>
+      </c>
+      <c r="E52" s="0" t="n">
+        <v>5581</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="B53" s="6" t="s">
+      <c r="A53" s="6" t="s">
         <v>108</v>
       </c>
-      <c r="C53" s="4" t="s">
-        <v>6</v>
+      <c r="B53" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="C53" s="5" t="s">
+        <v>7</v>
       </c>
       <c r="D53" s="0" t="n">
-        <v>180960</v>
+        <v>15100</v>
+      </c>
+      <c r="E53" s="0" t="n">
+        <v>40617</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="5" t="s">
-        <v>109</v>
-      </c>
-      <c r="B54" s="6" t="s">
+      <c r="A54" s="6" t="s">
         <v>110</v>
       </c>
-      <c r="C54" s="4" t="s">
-        <v>6</v>
+      <c r="B54" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="C54" s="5" t="s">
+        <v>7</v>
       </c>
       <c r="D54" s="0" t="n">
-        <v>361984</v>
+        <v>78754</v>
+      </c>
+      <c r="E54" s="8" t="n">
+        <v>194664</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="5" t="s">
-        <v>111</v>
-      </c>
-      <c r="B55" s="6" t="s">
+      <c r="A55" s="6" t="s">
         <v>112</v>
       </c>
-      <c r="C55" s="4" t="s">
-        <v>6</v>
+      <c r="B55" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="C55" s="5" t="s">
+        <v>7</v>
       </c>
       <c r="D55" s="0" t="n">
-        <v>12304882</v>
+        <v>46800</v>
+      </c>
+      <c r="E55" s="0" t="n">
+        <v>106552</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="5" t="s">
-        <v>113</v>
-      </c>
-      <c r="B56" s="6" t="s">
+      <c r="A56" s="6" t="s">
         <v>114</v>
       </c>
-      <c r="C56" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D56" s="0" t="n">
-        <v>2066575</v>
+      <c r="B56" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="C56" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D56" s="8" t="n">
+        <v>8093</v>
+      </c>
+      <c r="E56" s="0" t="n">
+        <v>8093</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="5" t="s">
-        <v>115</v>
-      </c>
-      <c r="B57" s="6" t="s">
+      <c r="A57" s="6" t="s">
         <v>116</v>
       </c>
-      <c r="C57" s="4" t="s">
-        <v>6</v>
+      <c r="B57" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="C57" s="5" t="s">
+        <v>7</v>
       </c>
       <c r="D57" s="0" t="n">
-        <v>1775571</v>
+        <v>90005</v>
+      </c>
+      <c r="E57" s="0" t="n">
+        <v>1062872</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="5" t="s">
-        <v>117</v>
-      </c>
-      <c r="B58" s="6" t="s">
+      <c r="A58" s="6" t="s">
         <v>118</v>
       </c>
-      <c r="C58" s="4" t="s">
-        <v>6</v>
+      <c r="B58" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="C58" s="5" t="s">
+        <v>7</v>
       </c>
       <c r="D58" s="0" t="n">
-        <v>16488436</v>
+        <v>337372</v>
+      </c>
+      <c r="E58" s="0" t="n">
+        <v>539466</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="5" t="s">
-        <v>119</v>
-      </c>
-      <c r="B59" s="6" t="s">
+      <c r="A59" s="6" t="s">
         <v>120</v>
       </c>
-      <c r="C59" s="4" t="s">
-        <v>6</v>
+      <c r="B59" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="C59" s="5" t="s">
+        <v>7</v>
       </c>
       <c r="D59" s="0" t="n">
-        <v>1938855</v>
+        <v>323063</v>
+      </c>
+      <c r="E59" s="0" t="n">
+        <v>408141</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="5" t="s">
-        <v>121</v>
-      </c>
-      <c r="B60" s="6" t="s">
+      <c r="A60" s="6" t="s">
         <v>122</v>
       </c>
-      <c r="C60" s="4" t="s">
-        <v>6</v>
+      <c r="B60" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="C60" s="5" t="s">
+        <v>7</v>
       </c>
       <c r="D60" s="0" t="n">
-        <v>1506419</v>
+        <v>204061</v>
+      </c>
+      <c r="E60" s="0" t="n">
+        <v>249761</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="5" t="s">
-        <v>123</v>
-      </c>
-      <c r="B61" s="6" t="s">
+      <c r="A61" s="6" t="s">
         <v>124</v>
       </c>
-      <c r="C61" s="4" t="s">
-        <v>6</v>
+      <c r="B61" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="C61" s="5" t="s">
+        <v>7</v>
       </c>
       <c r="D61" s="0" t="n">
-        <v>655226</v>
+        <v>499202</v>
+      </c>
+      <c r="E61" s="0" t="n">
+        <v>694474</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="5" t="s">
-        <v>125</v>
-      </c>
-      <c r="B62" s="6" t="s">
+      <c r="A62" s="6" t="s">
         <v>126</v>
       </c>
-      <c r="C62" s="4" t="s">
-        <v>6</v>
+      <c r="B62" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="C62" s="5" t="s">
+        <v>7</v>
       </c>
       <c r="D62" s="0" t="n">
-        <v>4449307</v>
+        <v>226283</v>
+      </c>
+      <c r="E62" s="0" t="n">
+        <v>359666</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="5" t="s">
-        <v>127</v>
-      </c>
-      <c r="B63" s="6" t="s">
+      <c r="A63" s="6" t="s">
         <v>128</v>
       </c>
-      <c r="C63" s="4" t="s">
-        <v>6</v>
+      <c r="B63" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="C63" s="5" t="s">
+        <v>7</v>
       </c>
       <c r="D63" s="0" t="n">
-        <v>2640932</v>
+        <v>111262</v>
+      </c>
+      <c r="E63" s="0" t="n">
+        <v>132302</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="B64" s="6" t="s">
+      <c r="A64" s="6" t="s">
         <v>130</v>
       </c>
-      <c r="C64" s="4" t="s">
-        <v>6</v>
+      <c r="B64" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="C64" s="5" t="s">
+        <v>7</v>
       </c>
       <c r="D64" s="0" t="n">
-        <v>1653735</v>
+        <v>393216</v>
+      </c>
+      <c r="E64" s="0" t="n">
+        <v>765427</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="5" t="s">
-        <v>131</v>
-      </c>
-      <c r="B65" s="6" t="s">
+      <c r="A65" s="6" t="s">
         <v>132</v>
       </c>
-      <c r="C65" s="4" t="s">
-        <v>6</v>
+      <c r="B65" s="7" t="s">
+        <v>133</v>
+      </c>
+      <c r="C65" s="5" t="s">
+        <v>7</v>
       </c>
       <c r="D65" s="0" t="n">
-        <v>469288</v>
+        <v>142132</v>
+      </c>
+      <c r="E65" s="0" t="n">
+        <v>168074</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="5" t="s">
-        <v>133</v>
-      </c>
-      <c r="B66" s="6" t="s">
+      <c r="A66" s="6" t="s">
         <v>134</v>
       </c>
-      <c r="C66" s="4" t="s">
-        <v>6</v>
+      <c r="B66" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="C66" s="5" t="s">
+        <v>7</v>
       </c>
       <c r="D66" s="0" t="n">
-        <v>3653196</v>
+        <v>412776</v>
+      </c>
+      <c r="E66" s="0" t="n">
+        <v>471421</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="5" t="s">
-        <v>135</v>
-      </c>
-      <c r="B67" s="6" t="s">
+      <c r="A67" s="6" t="s">
         <v>136</v>
       </c>
-      <c r="C67" s="4" t="s">
-        <v>6</v>
+      <c r="B67" s="7" t="s">
+        <v>137</v>
+      </c>
+      <c r="C67" s="5" t="s">
+        <v>7</v>
       </c>
       <c r="D67" s="0" t="n">
-        <v>519495</v>
+        <v>3229473</v>
+      </c>
+      <c r="E67" s="0" t="n">
+        <v>3445814</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A68" s="5" t="s">
-        <v>137</v>
-      </c>
-      <c r="B68" s="6" t="s">
+      <c r="A68" s="6" t="s">
         <v>138</v>
       </c>
-      <c r="C68" s="4" t="s">
-        <v>6</v>
+      <c r="B68" s="7" t="s">
+        <v>139</v>
+      </c>
+      <c r="C68" s="5" t="s">
+        <v>7</v>
       </c>
       <c r="D68" s="0" t="n">
-        <v>5977012</v>
+        <v>690952</v>
+      </c>
+      <c r="E68" s="0" t="n">
+        <v>1180056</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A69" s="5" t="s">
-        <v>139</v>
-      </c>
-      <c r="B69" s="6" t="s">
+      <c r="A69" s="6" t="s">
         <v>140</v>
       </c>
-      <c r="C69" s="4" t="s">
-        <v>6</v>
+      <c r="B69" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="C69" s="5" t="s">
+        <v>7</v>
       </c>
       <c r="D69" s="0" t="n">
-        <v>19879506</v>
+        <v>180648</v>
+      </c>
+      <c r="E69" s="0" t="n">
+        <v>195190</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A70" s="5" t="s">
-        <v>141</v>
-      </c>
-      <c r="B70" s="6" t="s">
+      <c r="A70" s="6" t="s">
         <v>142</v>
       </c>
-      <c r="C70" s="4" t="s">
-        <v>6</v>
+      <c r="B70" s="7" t="s">
+        <v>143</v>
+      </c>
+      <c r="C70" s="5" t="s">
+        <v>7</v>
       </c>
       <c r="D70" s="0" t="n">
-        <v>5332682</v>
+        <v>303588</v>
+      </c>
+      <c r="E70" s="0" t="n">
+        <v>468821</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A71" s="5" t="s">
-        <v>143</v>
-      </c>
-      <c r="B71" s="6" t="s">
+      <c r="A71" s="6" t="s">
         <v>144</v>
       </c>
-      <c r="C71" s="4" t="s">
-        <v>6</v>
+      <c r="B71" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="C71" s="5" t="s">
+        <v>7</v>
       </c>
       <c r="D71" s="0" t="n">
-        <v>757264</v>
+        <v>47369</v>
+      </c>
+      <c r="E71" s="0" t="n">
+        <v>66056</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A72" s="5" t="s">
-        <v>145</v>
-      </c>
-      <c r="B72" s="6" t="s">
+      <c r="A72" s="6" t="s">
         <v>146</v>
       </c>
-      <c r="C72" s="4" t="s">
-        <v>6</v>
+      <c r="B72" s="7" t="s">
+        <v>147</v>
+      </c>
+      <c r="C72" s="5" t="s">
+        <v>7</v>
       </c>
       <c r="D72" s="0" t="n">
-        <v>2259927</v>
+        <v>216942</v>
+      </c>
+      <c r="E72" s="0" t="n">
+        <v>222969</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A73" s="5" t="s">
-        <v>147</v>
-      </c>
-      <c r="B73" s="6" t="s">
+      <c r="A73" s="6" t="s">
         <v>148</v>
       </c>
-      <c r="C73" s="4" t="s">
-        <v>6</v>
+      <c r="B73" s="7" t="s">
+        <v>149</v>
+      </c>
+      <c r="C73" s="5" t="s">
+        <v>7</v>
       </c>
       <c r="D73" s="0" t="n">
-        <v>182202</v>
+        <v>537165</v>
+      </c>
+      <c r="E73" s="0" t="n">
+        <v>823627</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A74" s="5" t="s">
-        <v>149</v>
-      </c>
-      <c r="B74" s="6" t="s">
+      <c r="A74" s="6" t="s">
         <v>150</v>
       </c>
-      <c r="C74" s="4" t="s">
-        <v>6</v>
+      <c r="B74" s="7" t="s">
+        <v>151</v>
+      </c>
+      <c r="C74" s="5" t="s">
+        <v>7</v>
       </c>
       <c r="D74" s="0" t="n">
-        <v>1842504</v>
+        <v>581971</v>
+      </c>
+      <c r="E74" s="0" t="n">
+        <v>610098</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A75" s="5" t="s">
-        <v>151</v>
-      </c>
-      <c r="B75" s="6" t="s">
+      <c r="A75" s="6" t="s">
         <v>152</v>
       </c>
-      <c r="C75" s="4" t="s">
-        <v>6</v>
+      <c r="B75" s="7" t="s">
+        <v>153</v>
+      </c>
+      <c r="C75" s="5" t="s">
+        <v>7</v>
       </c>
       <c r="D75" s="0" t="n">
-        <v>11127235</v>
+        <v>117118</v>
+      </c>
+      <c r="E75" s="0" t="n">
+        <v>124837</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A76" s="5" t="s">
-        <v>153</v>
-      </c>
-      <c r="B76" s="6" t="s">
+      <c r="A76" s="6" t="s">
         <v>154</v>
       </c>
-      <c r="C76" s="4" t="s">
-        <v>6</v>
+      <c r="B76" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="C76" s="5" t="s">
+        <v>7</v>
       </c>
       <c r="D76" s="0" t="n">
-        <v>4276104</v>
+        <v>121431</v>
+      </c>
+      <c r="E76" s="0" t="n">
+        <v>3578739</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A77" s="5" t="s">
-        <v>155</v>
-      </c>
-      <c r="B77" s="6" t="s">
+      <c r="A77" s="6" t="s">
         <v>156</v>
       </c>
-      <c r="C77" s="4" t="s">
-        <v>6</v>
+      <c r="B77" s="7" t="s">
+        <v>157</v>
+      </c>
+      <c r="C77" s="5" t="s">
+        <v>7</v>
       </c>
       <c r="D77" s="0" t="n">
-        <v>877999</v>
+        <v>331613</v>
+      </c>
+      <c r="E77" s="0" t="n">
+        <v>398875</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A78" s="5" t="s">
-        <v>157</v>
-      </c>
-      <c r="B78" s="6" t="s">
+      <c r="A78" s="6" t="s">
         <v>158</v>
       </c>
-      <c r="C78" s="4" t="s">
-        <v>6</v>
+      <c r="B78" s="7" t="s">
+        <v>159</v>
+      </c>
+      <c r="C78" s="5" t="s">
+        <v>7</v>
       </c>
       <c r="D78" s="0" t="n">
-        <v>17409710</v>
+        <v>12141</v>
+      </c>
+      <c r="E78" s="0" t="n">
+        <v>229957</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A79" s="5" t="s">
-        <v>159</v>
-      </c>
-      <c r="B79" s="6" t="s">
+      <c r="A79" s="6" t="s">
         <v>160</v>
       </c>
-      <c r="C79" s="4" t="s">
-        <v>6</v>
+      <c r="B79" s="7" t="s">
+        <v>161</v>
+      </c>
+      <c r="C79" s="5" t="s">
+        <v>7</v>
       </c>
       <c r="D79" s="0" t="n">
-        <v>3574695</v>
+        <v>16505</v>
+      </c>
+      <c r="E79" s="0" t="n">
+        <v>25072</v>
+      </c>
+      <c r="F79" s="0" t="s">
+        <v>162</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A80" s="5" t="s">
-        <v>161</v>
-      </c>
-      <c r="B80" s="6" t="s">
-        <v>162</v>
-      </c>
-      <c r="C80" s="4" t="s">
-        <v>6</v>
+      <c r="A80" s="6" t="s">
+        <v>163</v>
+      </c>
+      <c r="B80" s="7" t="s">
+        <v>164</v>
+      </c>
+      <c r="C80" s="5" t="s">
+        <v>7</v>
       </c>
       <c r="D80" s="0" t="n">
-        <v>2706534</v>
+        <v>342205</v>
+      </c>
+      <c r="E80" s="0" t="n">
+        <v>414574</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A81" s="5" t="s">
-        <v>163</v>
-      </c>
-      <c r="B81" s="6" t="s">
-        <v>164</v>
-      </c>
-      <c r="C81" s="4" t="s">
-        <v>6</v>
+      <c r="A81" s="6" t="s">
+        <v>165</v>
+      </c>
+      <c r="B81" s="7" t="s">
+        <v>166</v>
+      </c>
+      <c r="C81" s="5" t="s">
+        <v>7</v>
       </c>
       <c r="D81" s="0" t="n">
-        <v>158939</v>
+        <v>177003</v>
+      </c>
+      <c r="E81" s="0" t="n">
+        <v>305805</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A82" s="5" t="s">
-        <v>165</v>
-      </c>
-      <c r="B82" s="6" t="s">
-        <v>166</v>
-      </c>
-      <c r="C82" s="4" t="s">
-        <v>6</v>
+      <c r="A82" s="6" t="s">
+        <v>167</v>
+      </c>
+      <c r="B82" s="7" t="s">
+        <v>168</v>
+      </c>
+      <c r="C82" s="5" t="s">
+        <v>7</v>
       </c>
       <c r="D82" s="0" t="n">
-        <v>3482695</v>
+        <v>19209</v>
+      </c>
+      <c r="E82" s="0" t="n">
+        <v>26981</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A83" s="5" t="s">
-        <v>167</v>
-      </c>
-      <c r="B83" s="6" t="s">
-        <v>168</v>
-      </c>
-      <c r="C83" s="4" t="s">
-        <v>6</v>
+      <c r="A83" s="6" t="s">
+        <v>169</v>
+      </c>
+      <c r="B83" s="7" t="s">
+        <v>170</v>
+      </c>
+      <c r="C83" s="5" t="s">
+        <v>7</v>
       </c>
       <c r="D83" s="0" t="n">
-        <v>1464958</v>
+        <v>13924</v>
+      </c>
+      <c r="E83" s="0" t="n">
+        <v>24467</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A84" s="5" t="s">
-        <v>169</v>
-      </c>
-      <c r="B84" s="6" t="s">
-        <v>170</v>
-      </c>
-      <c r="C84" s="4" t="s">
-        <v>6</v>
+      <c r="A84" s="6" t="s">
+        <v>171</v>
+      </c>
+      <c r="B84" s="7" t="s">
+        <v>172</v>
+      </c>
+      <c r="C84" s="5" t="s">
+        <v>7</v>
       </c>
       <c r="D84" s="0" t="n">
-        <v>97198</v>
+        <v>2829</v>
+      </c>
+      <c r="E84" s="0" t="n">
+        <v>2936</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A85" s="5" t="s">
-        <v>171</v>
-      </c>
-      <c r="B85" s="6" t="s">
-        <v>172</v>
-      </c>
-      <c r="C85" s="4" t="s">
-        <v>6</v>
+      <c r="A85" s="6" t="s">
+        <v>173</v>
+      </c>
+      <c r="B85" s="7" t="s">
+        <v>174</v>
+      </c>
+      <c r="C85" s="5" t="s">
+        <v>7</v>
       </c>
       <c r="D85" s="0" t="n">
-        <v>54228</v>
+        <v>20660</v>
+      </c>
+      <c r="E85" s="0" t="n">
+        <v>28713</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A86" s="5" t="s">
-        <v>173</v>
-      </c>
-      <c r="B86" s="6" t="s">
-        <v>174</v>
-      </c>
-      <c r="C86" s="4" t="s">
-        <v>6</v>
+      <c r="A86" s="6" t="s">
+        <v>175</v>
+      </c>
+      <c r="B86" s="7" t="s">
+        <v>176</v>
+      </c>
+      <c r="C86" s="5" t="s">
+        <v>7</v>
       </c>
       <c r="D86" s="0" t="n">
-        <v>211995</v>
+        <v>56913</v>
+      </c>
+      <c r="E86" s="0" t="n">
+        <v>77526</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A87" s="5" t="s">
-        <v>175</v>
-      </c>
-      <c r="B87" s="6" t="s">
-        <v>176</v>
-      </c>
-      <c r="C87" s="4" t="s">
-        <v>6</v>
+      <c r="A87" s="6" t="s">
+        <v>177</v>
+      </c>
+      <c r="B87" s="7" t="s">
+        <v>178</v>
+      </c>
+      <c r="C87" s="5" t="s">
+        <v>7</v>
       </c>
       <c r="D87" s="0" t="n">
-        <v>4745897</v>
+        <v>48226</v>
+      </c>
+      <c r="E87" s="0" t="n">
+        <v>90508</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A88" s="5" t="s">
-        <v>177</v>
-      </c>
-      <c r="B88" s="6" t="s">
-        <v>178</v>
-      </c>
-      <c r="C88" s="4" t="s">
-        <v>6</v>
+      <c r="A88" s="6" t="s">
+        <v>179</v>
+      </c>
+      <c r="B88" s="7" t="s">
+        <v>180</v>
+      </c>
+      <c r="C88" s="5" t="s">
+        <v>7</v>
       </c>
       <c r="D88" s="0" t="n">
-        <v>126798</v>
+        <v>77103</v>
+      </c>
+      <c r="E88" s="0" t="n">
+        <v>95242</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A89" s="5" t="s">
-        <v>179</v>
-      </c>
-      <c r="B89" s="6" t="s">
-        <v>180</v>
-      </c>
-      <c r="C89" s="4" t="s">
-        <v>6</v>
+      <c r="A89" s="6" t="s">
+        <v>181</v>
+      </c>
+      <c r="B89" s="7" t="s">
+        <v>182</v>
+      </c>
+      <c r="C89" s="5" t="s">
+        <v>7</v>
       </c>
       <c r="D89" s="0" t="n">
-        <v>819351</v>
+        <v>21721</v>
+      </c>
+      <c r="E89" s="0" t="n">
+        <v>97438</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A90" s="5" t="s">
-        <v>181</v>
-      </c>
-      <c r="B90" s="6" t="s">
-        <v>182</v>
-      </c>
-      <c r="C90" s="4" t="s">
-        <v>6</v>
+      <c r="A90" s="6" t="s">
+        <v>183</v>
+      </c>
+      <c r="B90" s="7" t="s">
+        <v>184</v>
+      </c>
+      <c r="C90" s="5" t="s">
+        <v>7</v>
       </c>
       <c r="D90" s="0" t="n">
-        <v>1695980</v>
+        <v>49071</v>
+      </c>
+      <c r="E90" s="0" t="n">
+        <v>94544</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A91" s="5" t="s">
-        <v>183</v>
-      </c>
-      <c r="B91" s="6" t="s">
-        <v>184</v>
-      </c>
-      <c r="C91" s="4" t="s">
-        <v>6</v>
+      <c r="A91" s="6" t="s">
+        <v>185</v>
+      </c>
+      <c r="B91" s="7" t="s">
+        <v>186</v>
+      </c>
+      <c r="C91" s="5" t="s">
+        <v>7</v>
       </c>
       <c r="D91" s="0" t="n">
-        <v>1100255</v>
+        <v>30932</v>
+      </c>
+      <c r="E91" s="0" t="n">
+        <v>35155</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A92" s="5" t="s">
-        <v>185</v>
-      </c>
-      <c r="B92" s="6" t="s">
-        <v>186</v>
-      </c>
-      <c r="C92" s="4" t="s">
-        <v>6</v>
+      <c r="A92" s="6" t="s">
+        <v>187</v>
+      </c>
+      <c r="B92" s="7" t="s">
+        <v>188</v>
+      </c>
+      <c r="C92" s="5" t="s">
+        <v>7</v>
       </c>
       <c r="D92" s="0" t="n">
-        <v>1903313</v>
+        <v>36396</v>
+      </c>
+      <c r="E92" s="0" t="n">
+        <v>350473</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A93" s="5" t="s">
-        <v>187</v>
-      </c>
-      <c r="B93" s="6" t="s">
-        <v>188</v>
-      </c>
-      <c r="C93" s="4" t="s">
-        <v>6</v>
+      <c r="A93" s="6" t="s">
+        <v>189</v>
+      </c>
+      <c r="B93" s="7" t="s">
+        <v>190</v>
+      </c>
+      <c r="C93" s="5" t="s">
+        <v>7</v>
       </c>
       <c r="D93" s="0" t="n">
-        <v>2614240</v>
+        <v>81385</v>
+      </c>
+      <c r="E93" s="0" t="n">
+        <v>115855</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A94" s="5" t="s">
-        <v>189</v>
-      </c>
-      <c r="B94" s="6" t="s">
-        <v>190</v>
-      </c>
-      <c r="C94" s="4" t="s">
-        <v>6</v>
+      <c r="A94" s="6" t="s">
+        <v>191</v>
+      </c>
+      <c r="B94" s="7" t="s">
+        <v>192</v>
+      </c>
+      <c r="C94" s="5" t="s">
+        <v>7</v>
       </c>
       <c r="D94" s="0" t="n">
-        <v>1618167</v>
+        <v>0</v>
+      </c>
+      <c r="E94" s="0" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A95" s="5" t="s">
-        <v>191</v>
-      </c>
-      <c r="B95" s="6" t="s">
-        <v>192</v>
-      </c>
-      <c r="C95" s="4" t="s">
-        <v>6</v>
+      <c r="A95" s="6" t="s">
+        <v>193</v>
+      </c>
+      <c r="B95" s="7" t="s">
+        <v>194</v>
+      </c>
+      <c r="C95" s="5" t="s">
+        <v>7</v>
       </c>
       <c r="D95" s="0" t="n">
-        <v>1459103</v>
+        <v>2870520</v>
+      </c>
+      <c r="E95" s="0" t="n">
+        <v>4314597</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A96" s="5" t="s">
-        <v>193</v>
-      </c>
-      <c r="B96" s="6" t="s">
-        <v>194</v>
-      </c>
-      <c r="C96" s="4" t="s">
-        <v>6</v>
+      <c r="A96" s="6" t="s">
+        <v>195</v>
+      </c>
+      <c r="B96" s="7" t="s">
+        <v>196</v>
+      </c>
+      <c r="C96" s="5" t="s">
+        <v>7</v>
       </c>
       <c r="D96" s="0" t="n">
-        <v>7973723</v>
+        <v>9184582</v>
+      </c>
+      <c r="E96" s="0" t="n">
+        <v>26161303</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A97" s="5" t="s">
-        <v>195</v>
-      </c>
-      <c r="B97" s="6" t="s">
-        <v>196</v>
-      </c>
-      <c r="C97" s="4" t="s">
-        <v>6</v>
+      <c r="A97" s="6" t="s">
+        <v>197</v>
+      </c>
+      <c r="B97" s="7" t="s">
+        <v>198</v>
+      </c>
+      <c r="C97" s="5" t="s">
+        <v>7</v>
       </c>
       <c r="D97" s="0" t="n">
-        <v>4490440</v>
+        <v>72900</v>
+      </c>
+      <c r="E97" s="0" t="n">
+        <v>135678</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A98" s="5" t="s">
-        <v>197</v>
-      </c>
-      <c r="B98" s="6" t="s">
-        <v>198</v>
-      </c>
-      <c r="C98" s="4" t="s">
-        <v>6</v>
+      <c r="A98" s="6" t="s">
+        <v>199</v>
+      </c>
+      <c r="B98" s="7" t="s">
+        <v>200</v>
+      </c>
+      <c r="C98" s="5" t="s">
+        <v>7</v>
       </c>
       <c r="D98" s="0" t="n">
-        <v>9743082</v>
+        <v>770433</v>
+      </c>
+      <c r="E98" s="0" t="n">
+        <v>913193</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A99" s="5" t="s">
-        <v>199</v>
-      </c>
-      <c r="B99" s="6" t="s">
-        <v>200</v>
-      </c>
-      <c r="C99" s="4" t="s">
-        <v>6</v>
+      <c r="A99" s="6" t="s">
+        <v>201</v>
+      </c>
+      <c r="B99" s="7" t="s">
+        <v>202</v>
+      </c>
+      <c r="C99" s="5" t="s">
+        <v>7</v>
       </c>
       <c r="D99" s="0" t="n">
-        <v>3664092</v>
+        <v>657208</v>
+      </c>
+      <c r="E99" s="0" t="n">
+        <v>1109317</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A100" s="5" t="s">
-        <v>201</v>
-      </c>
-      <c r="B100" s="6" t="s">
-        <v>202</v>
-      </c>
-      <c r="C100" s="4" t="s">
-        <v>6</v>
+      <c r="A100" s="6" t="s">
+        <v>203</v>
+      </c>
+      <c r="B100" s="7" t="s">
+        <v>204</v>
+      </c>
+      <c r="C100" s="5" t="s">
+        <v>7</v>
       </c>
       <c r="D100" s="0" t="n">
-        <v>2291550</v>
+        <v>43315</v>
+      </c>
+      <c r="E100" s="0" t="n">
+        <v>82559</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A101" s="5" t="s">
-        <v>203</v>
-      </c>
-      <c r="B101" s="6" t="s">
-        <v>204</v>
-      </c>
-      <c r="C101" s="4" t="s">
-        <v>6</v>
+      <c r="A101" s="6" t="s">
+        <v>205</v>
+      </c>
+      <c r="B101" s="7" t="s">
+        <v>206</v>
+      </c>
+      <c r="C101" s="5" t="s">
+        <v>7</v>
       </c>
       <c r="D101" s="0" t="n">
-        <v>1957614</v>
+        <v>1546712</v>
+      </c>
+      <c r="E101" s="0" t="n">
+        <v>482899</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A102" s="5" t="s">
-        <v>205</v>
-      </c>
-      <c r="B102" s="6" t="s">
-        <v>206</v>
-      </c>
-      <c r="C102" s="4" t="s">
-        <v>6</v>
+      <c r="A102" s="6" t="s">
+        <v>207</v>
+      </c>
+      <c r="B102" s="7" t="s">
+        <v>208</v>
+      </c>
+      <c r="C102" s="5" t="s">
+        <v>7</v>
       </c>
       <c r="D102" s="0" t="n">
-        <v>3455099</v>
+        <v>125514</v>
+      </c>
+      <c r="E102" s="0" t="n">
+        <v>161178</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A103" s="5" t="s">
-        <v>207</v>
-      </c>
-      <c r="B103" s="6" t="s">
-        <v>208</v>
-      </c>
-      <c r="C103" s="4" t="s">
-        <v>6</v>
+      <c r="A103" s="6" t="s">
+        <v>209</v>
+      </c>
+      <c r="B103" s="7" t="s">
+        <v>210</v>
+      </c>
+      <c r="C103" s="5" t="s">
+        <v>7</v>
       </c>
       <c r="D103" s="0" t="n">
-        <v>3004533</v>
+        <v>178613</v>
+      </c>
+      <c r="E103" s="0" t="n">
+        <v>302368</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A104" s="5" t="s">
-        <v>209</v>
-      </c>
-      <c r="B104" s="6" t="s">
-        <v>210</v>
-      </c>
-      <c r="C104" s="4" t="s">
-        <v>6</v>
+      <c r="A104" s="6" t="s">
+        <v>211</v>
+      </c>
+      <c r="B104" s="7" t="s">
+        <v>212</v>
+      </c>
+      <c r="C104" s="5" t="s">
+        <v>7</v>
       </c>
       <c r="D104" s="0" t="n">
-        <v>1546712</v>
+        <v>226051</v>
+      </c>
+      <c r="E104" s="0" t="n">
+        <v>430956</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A105" s="5" t="s">
-        <v>211</v>
-      </c>
-      <c r="B105" s="6" t="s">
-        <v>212</v>
-      </c>
-      <c r="C105" s="4" t="s">
-        <v>6</v>
+      <c r="A105" s="6" t="s">
+        <v>213</v>
+      </c>
+      <c r="B105" s="7" t="s">
+        <v>214</v>
+      </c>
+      <c r="C105" s="5" t="s">
+        <v>7</v>
       </c>
       <c r="D105" s="0" t="n">
-        <v>451029</v>
+        <v>109956</v>
+      </c>
+      <c r="E105" s="0" t="n">
+        <v>304547</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A106" s="5" t="s">
-        <v>213</v>
-      </c>
-      <c r="B106" s="6" t="s">
-        <v>214</v>
-      </c>
-      <c r="C106" s="4" t="s">
-        <v>6</v>
+      <c r="A106" s="6" t="s">
+        <v>215</v>
+      </c>
+      <c r="B106" s="7" t="s">
+        <v>216</v>
+      </c>
+      <c r="C106" s="5" t="s">
+        <v>7</v>
       </c>
       <c r="D106" s="0" t="n">
-        <v>1477680</v>
+        <v>18477</v>
+      </c>
+      <c r="E106" s="0" t="n">
+        <v>18853</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A107" s="5" t="s">
-        <v>215</v>
-      </c>
-      <c r="B107" s="6" t="s">
-        <v>216</v>
-      </c>
-      <c r="C107" s="4" t="s">
-        <v>6</v>
+      <c r="A107" s="6" t="s">
+        <v>217</v>
+      </c>
+      <c r="B107" s="7" t="s">
+        <v>218</v>
+      </c>
+      <c r="C107" s="5" t="s">
+        <v>7</v>
       </c>
       <c r="D107" s="0" t="n">
-        <v>1744569</v>
+        <v>92163</v>
+      </c>
+      <c r="E107" s="0" t="n">
+        <v>98882</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A108" s="5" t="s">
-        <v>217</v>
-      </c>
-      <c r="B108" s="6" t="s">
-        <v>218</v>
-      </c>
-      <c r="C108" s="4" t="s">
-        <v>6</v>
+      <c r="A108" s="6" t="s">
+        <v>219</v>
+      </c>
+      <c r="B108" s="7" t="s">
+        <v>220</v>
+      </c>
+      <c r="C108" s="5" t="s">
+        <v>7</v>
       </c>
       <c r="D108" s="0" t="n">
-        <v>894687</v>
+        <v>231877</v>
+      </c>
+      <c r="E108" s="0" t="n">
+        <v>302267</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A109" s="5" t="s">
-        <v>219</v>
-      </c>
-      <c r="B109" s="6" t="s">
-        <v>220</v>
-      </c>
-      <c r="C109" s="4" t="s">
-        <v>6</v>
+      <c r="A109" s="6" t="s">
+        <v>221</v>
+      </c>
+      <c r="B109" s="7" t="s">
+        <v>222</v>
+      </c>
+      <c r="C109" s="5" t="s">
+        <v>7</v>
       </c>
       <c r="D109" s="0" t="n">
-        <v>69900</v>
+        <v>10002</v>
+      </c>
+      <c r="E109" s="0" t="n">
+        <v>24500</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A110" s="5" t="s">
-        <v>221</v>
-      </c>
-      <c r="B110" s="6" t="s">
-        <v>222</v>
-      </c>
-      <c r="C110" s="4" t="s">
-        <v>6</v>
+      <c r="A110" s="6" t="s">
+        <v>223</v>
+      </c>
+      <c r="B110" s="7" t="s">
+        <v>224</v>
+      </c>
+      <c r="C110" s="5" t="s">
+        <v>7</v>
       </c>
       <c r="D110" s="0" t="n">
-        <v>920486</v>
+        <v>63139</v>
+      </c>
+      <c r="E110" s="0" t="n">
+        <v>117838</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A111" s="5" t="s">
-        <v>223</v>
-      </c>
-      <c r="B111" s="6" t="s">
-        <v>224</v>
-      </c>
-      <c r="C111" s="4" t="s">
-        <v>6</v>
+      <c r="A111" s="6" t="s">
+        <v>225</v>
+      </c>
+      <c r="B111" s="7" t="s">
+        <v>226</v>
+      </c>
+      <c r="C111" s="5" t="s">
+        <v>7</v>
       </c>
       <c r="D111" s="0" t="n">
-        <v>2244792</v>
+        <v>358992</v>
+      </c>
+      <c r="E111" s="0" t="n">
+        <v>764956</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A112" s="5" t="s">
-        <v>225</v>
-      </c>
-      <c r="B112" s="6" t="s">
-        <v>226</v>
-      </c>
-      <c r="C112" s="4" t="s">
-        <v>6</v>
+      <c r="A112" s="6" t="s">
+        <v>227</v>
+      </c>
+      <c r="B112" s="7" t="s">
+        <v>228</v>
+      </c>
+      <c r="C112" s="5" t="s">
+        <v>7</v>
       </c>
       <c r="D112" s="0" t="n">
-        <v>67449</v>
+        <v>117992</v>
+      </c>
+      <c r="E112" s="0" t="n">
+        <v>187235</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A113" s="5" t="s">
-        <v>227</v>
-      </c>
-      <c r="B113" s="6" t="s">
-        <v>228</v>
-      </c>
-      <c r="C113" s="4" t="s">
-        <v>6</v>
+      <c r="A113" s="6" t="s">
+        <v>229</v>
+      </c>
+      <c r="B113" s="7" t="s">
+        <v>230</v>
+      </c>
+      <c r="C113" s="5" t="s">
+        <v>7</v>
       </c>
       <c r="D113" s="0" t="n">
-        <v>595075</v>
+        <v>155698</v>
+      </c>
+      <c r="E113" s="0" t="n">
+        <v>174715</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A114" s="5" t="s">
-        <v>229</v>
-      </c>
-      <c r="B114" s="6" t="s">
-        <v>230</v>
-      </c>
-      <c r="C114" s="4" t="s">
-        <v>6</v>
+      <c r="A114" s="6" t="s">
+        <v>231</v>
+      </c>
+      <c r="B114" s="7" t="s">
+        <v>232</v>
+      </c>
+      <c r="C114" s="5" t="s">
+        <v>7</v>
       </c>
       <c r="D114" s="0" t="n">
-        <v>6221437</v>
+        <v>10226</v>
+      </c>
+      <c r="E114" s="0" t="n">
+        <v>237624</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A115" s="5" t="s">
-        <v>231</v>
-      </c>
-      <c r="B115" s="6" t="s">
-        <v>232</v>
-      </c>
-      <c r="C115" s="4" t="s">
-        <v>6</v>
+      <c r="A115" s="6" t="s">
+        <v>233</v>
+      </c>
+      <c r="B115" s="7" t="s">
+        <v>234</v>
+      </c>
+      <c r="C115" s="5" t="s">
+        <v>7</v>
       </c>
       <c r="D115" s="0" t="n">
-        <v>1197675</v>
+        <v>193959</v>
+      </c>
+      <c r="E115" s="0" t="n">
+        <v>200263</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A116" s="5" t="s">
-        <v>233</v>
-      </c>
-      <c r="B116" s="6" t="s">
-        <v>234</v>
-      </c>
-      <c r="C116" s="4" t="s">
-        <v>6</v>
+      <c r="A116" s="6" t="s">
+        <v>235</v>
+      </c>
+      <c r="B116" s="7" t="s">
+        <v>236</v>
+      </c>
+      <c r="C116" s="5" t="s">
+        <v>7</v>
       </c>
       <c r="D116" s="0" t="n">
-        <v>1773346</v>
+        <v>326</v>
+      </c>
+      <c r="E116" s="0" t="n">
+        <v>913</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A117" s="5" t="s">
-        <v>235</v>
-      </c>
-      <c r="B117" s="6" t="s">
-        <v>236</v>
-      </c>
-      <c r="C117" s="4" t="s">
-        <v>6</v>
+      <c r="A117" s="0" t="s">
+        <v>237</v>
+      </c>
+      <c r="B117" s="0" t="s">
+        <v>238</v>
+      </c>
+      <c r="C117" s="0" t="s">
+        <v>7</v>
       </c>
       <c r="D117" s="0" t="n">
-        <v>6158626</v>
-      </c>
-    </row>
-    <row r="118" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A118" s="5" t="s">
-        <v>237</v>
-      </c>
-      <c r="B118" s="6" t="s">
-        <v>238</v>
-      </c>
-      <c r="C118" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D118" s="0" t="n">
-        <v>738239</v>
-      </c>
-    </row>
-    <row r="119" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A119" s="5" t="s">
-        <v>239</v>
-      </c>
-      <c r="B119" s="6" t="s">
-        <v>240</v>
-      </c>
-      <c r="C119" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D119" s="0" t="n">
-        <v>896088</v>
+        <v>28948</v>
+      </c>
+      <c r="E117" s="0" t="n">
+        <v>106119</v>
       </c>
     </row>
   </sheetData>

</xml_diff>